<commit_message>
did some more data analysis found shannons diversity H = 1.86 V. low pollinator diversity need to figure out how to remove the NA column in my plot
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teddy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonhi\OneDrive\Desktop\WCU\2.F22\COAD-Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA99B15-DE50-4CBA-A21E-CC3DE1FA5875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD5DAB6-23C0-4FF2-880C-420A88157B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5DDF21AA-DF19-4001-BAD9-28C5D5C88F9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5DDF21AA-DF19-4001-BAD9-28C5D5C88F9B}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="56">
   <si>
     <t>Group Name</t>
   </si>
@@ -186,6 +186,24 @@
   <si>
     <t>replicates</t>
   </si>
+  <si>
+    <t>pi</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>ln(pi)</t>
+  </si>
+  <si>
+    <t>pi(ln)pi</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
@@ -228,7 +246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -244,6 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -251,6 +270,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00CC00"/>
+      <color rgb="FF99CC00"/>
+      <color rgb="FFCCFF33"/>
+      <color rgb="FF00CC99"/>
+      <color rgb="FFFF33CC"/>
+      <color rgb="FFCC66FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -561,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE60CD1B-DD73-433B-99A1-C6264EFA5C69}">
   <dimension ref="A1:G381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A343" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6714,17 +6743,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5541F0C9-B269-4B59-9D76-579C7804CF57}">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection sqref="A1:L39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
-    <col min="3" max="12" width="9.140625" style="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="11" style="1" customWidth="1"/>
+    <col min="10" max="12" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -7943,7 +7976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -7981,7 +8014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -8019,7 +8052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -8057,7 +8090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
@@ -8095,7 +8128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
@@ -8133,7 +8166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>31</v>
       </c>
@@ -8171,7 +8204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>31</v>
       </c>
@@ -8207,6 +8240,215 @@
       </c>
       <c r="L39" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C42" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" s="1">
+        <f>SUM(D2:D39)</f>
+        <v>310</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" ref="E42:L42" si="0">SUM(E2:E39)</f>
+        <v>165</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="0"/>
+        <v>222</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="H42" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="I42" s="1">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="J42" s="1">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="K42" s="1">
+        <f t="shared" si="0"/>
+        <v>191</v>
+      </c>
+      <c r="L42" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M42" s="1">
+        <f>SUM(D42:L42)</f>
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C43" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" s="1">
+        <f>D42/$M42</f>
+        <v>0.272887323943662</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" ref="E43:L43" si="1">E42/$M42</f>
+        <v>0.14524647887323944</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="1"/>
+        <v>0.1954225352112676</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="1"/>
+        <v>8.1866197183098594E-2</v>
+      </c>
+      <c r="H43" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1443661971830986E-2</v>
+      </c>
+      <c r="I43" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5774647887323945E-2</v>
+      </c>
+      <c r="J43" s="1">
+        <f t="shared" si="1"/>
+        <v>7.8345070422535218E-2</v>
+      </c>
+      <c r="K43" s="1">
+        <f t="shared" si="1"/>
+        <v>0.16813380281690141</v>
+      </c>
+      <c r="L43" s="1">
+        <f t="shared" si="1"/>
+        <v>8.8028169014084509E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C44" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="1">
+        <f>LN(D43)</f>
+        <v>-1.2986963018019047</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" ref="E44:K44" si="2">LN(E43)</f>
+        <v>-1.9293231253805161</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.6325912174088173</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="2"/>
+        <v>-2.5026691061278408</v>
+      </c>
+      <c r="H44" s="1">
+        <f t="shared" si="2"/>
+        <v>-4.4703192418195599</v>
+      </c>
+      <c r="I44" s="1">
+        <f t="shared" si="2"/>
+        <v>-3.0840248806996691</v>
+      </c>
+      <c r="J44" s="1">
+        <f t="shared" si="2"/>
+        <v>-2.5466322295489565</v>
+      </c>
+      <c r="K44" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.7829951712344667</v>
+      </c>
+      <c r="L44" s="1">
+        <f>LN(L43)</f>
+        <v>-7.035268599281097</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C45" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" s="1">
+        <f>D43*D44</f>
+        <v>-0.3543977584142522</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" ref="E45:L45" si="3">E43*E44</f>
+        <v>-0.28022739057023344</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.31904511466968083</v>
+      </c>
+      <c r="G45" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.20488400252631092</v>
+      </c>
+      <c r="H45" s="1">
+        <f t="shared" si="3"/>
+        <v>-5.1156822309554824E-2</v>
+      </c>
+      <c r="I45" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.14117015298977359</v>
+      </c>
+      <c r="J45" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.19951608136431087</v>
+      </c>
+      <c r="K45" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.29978175854382316</v>
+      </c>
+      <c r="L45" s="1">
+        <f t="shared" si="3"/>
+        <v>-6.19301813316998E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C47" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="9">
+        <f>-SUM(D45:L45)</f>
+        <v>1.8563720995211099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>